<commit_message>
Changes and new goblin shop item
</commit_message>
<xml_diff>
--- a/resources/data-imports/Items/alchemy-items.xlsx
+++ b/resources/data-imports/Items/alchemy-items.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="335">
   <si>
     <t>id</t>
   </si>
@@ -1014,6 +1014,12 @@
   </si>
   <si>
     <t>This stew smells disgusting. It even tastes like you are being posioned and about to die. However the effects of this are felt instantly in battle.</t>
+  </si>
+  <si>
+    <t>Scroll of forbidden rights</t>
+  </si>
+  <si>
+    <t>A scroll that grants the user the rights of the forbidden children of Alicatar. A sacred realm of Ascension.</t>
   </si>
 </sst>
 </file>
@@ -1353,7 +1359,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BT127"/>
+  <dimension ref="A1:BT128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1361,7 +1367,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.141" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="37.705" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
@@ -16743,7 +16749,7 @@
     </row>
     <row r="127" spans="1:72">
       <c r="A127">
-        <v>938223</v>
+        <v>1094934</v>
       </c>
       <c r="C127" t="s">
         <v>331</v>
@@ -16754,6 +16760,9 @@
       <c r="G127" t="s">
         <v>332</v>
       </c>
+      <c r="O127">
+        <v>0</v>
+      </c>
       <c r="P127">
         <v>5000</v>
       </c>
@@ -16766,14 +16775,38 @@
       <c r="S127">
         <v>0.75</v>
       </c>
+      <c r="Y127">
+        <v>0</v>
+      </c>
+      <c r="Z127">
+        <v>0</v>
+      </c>
       <c r="AC127">
         <v>1</v>
       </c>
+      <c r="AI127">
+        <v>0</v>
+      </c>
+      <c r="AJ127">
+        <v>0</v>
+      </c>
+      <c r="AK127">
+        <v>0</v>
+      </c>
+      <c r="AL127">
+        <v>0</v>
+      </c>
+      <c r="AM127">
+        <v>0</v>
+      </c>
       <c r="AP127">
         <v>1</v>
       </c>
       <c r="AQ127">
         <v>1</v>
+      </c>
+      <c r="AS127">
+        <v>0</v>
       </c>
       <c r="AT127">
         <v>120</v>
@@ -16784,6 +16817,33 @@
       <c r="AV127">
         <v>1.2</v>
       </c>
+      <c r="AX127">
+        <v>0</v>
+      </c>
+      <c r="AY127">
+        <v>0</v>
+      </c>
+      <c r="BA127">
+        <v>0</v>
+      </c>
+      <c r="BB127">
+        <v>0</v>
+      </c>
+      <c r="BC127">
+        <v>0</v>
+      </c>
+      <c r="BD127">
+        <v>0</v>
+      </c>
+      <c r="BE127">
+        <v>0</v>
+      </c>
+      <c r="BF127">
+        <v>0</v>
+      </c>
+      <c r="BG127">
+        <v>0</v>
+      </c>
       <c r="BI127">
         <v>15</v>
       </c>
@@ -16806,6 +16866,74 @@
         <v>0</v>
       </c>
       <c r="BR127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:72">
+      <c r="A128">
+        <v>1095245</v>
+      </c>
+      <c r="C128" t="s">
+        <v>333</v>
+      </c>
+      <c r="D128" t="s">
+        <v>73</v>
+      </c>
+      <c r="G128" t="s">
+        <v>334</v>
+      </c>
+      <c r="P128">
+        <v>7500</v>
+      </c>
+      <c r="Q128">
+        <v>1.5</v>
+      </c>
+      <c r="R128">
+        <v>1</v>
+      </c>
+      <c r="S128">
+        <v>1.25</v>
+      </c>
+      <c r="AC128">
+        <v>1</v>
+      </c>
+      <c r="AP128">
+        <v>1</v>
+      </c>
+      <c r="AQ128">
+        <v>1</v>
+      </c>
+      <c r="AT128">
+        <v>240</v>
+      </c>
+      <c r="AU128">
+        <v>1</v>
+      </c>
+      <c r="AV128">
+        <v>1.75</v>
+      </c>
+      <c r="BI128">
+        <v>3</v>
+      </c>
+      <c r="BJ128">
+        <v>1</v>
+      </c>
+      <c r="BM128">
+        <v>0</v>
+      </c>
+      <c r="BN128">
+        <v>0</v>
+      </c>
+      <c r="BO128">
+        <v>0</v>
+      </c>
+      <c r="BP128">
+        <v>0</v>
+      </c>
+      <c r="BQ128">
+        <v>0</v>
+      </c>
+      <c r="BR128">
         <v>1</v>
       </c>
     </row>

</xml_diff>